<commit_message>
chore: update planning marqueurs 2023
</commit_message>
<xml_diff>
--- a/planning_marqueurs_2023.xlsx
+++ b/planning_marqueurs_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielkostro/git/github/stropitek/lvbc-scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B668F4A-0366-4643-B43B-69D5D4EF4FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CD720D-77FA-DE40-8BAE-366C9C4F5B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,7 +431,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -442,6 +446,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0CE31C4F-0141-C041-9E11-411F47CE4252}" name="Table1" displayName="Table1" ref="A1:K83" totalsRowShown="0">
+  <autoFilter ref="A1:K83" xr:uid="{0CE31C4F-0141-C041-9E11-411F47CE4252}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{5DBCBA35-60EE-E44F-876F-615D9FD3E12A}" name="# Match"/>
+    <tableColumn id="2" xr3:uid="{E7D62CCE-13D3-A54D-9BD5-FFB881CB982B}" name="H/F"/>
+    <tableColumn id="3" xr3:uid="{6CBCD0E3-7358-8E44-98E1-B7F3DAF0E7F5}" name="CL"/>
+    <tableColumn id="4" xr3:uid="{9D9A18E9-7D2C-1D42-BC95-52D14AE2000D}" name="Ligue"/>
+    <tableColumn id="5" xr3:uid="{31EA02A8-B7D3-7646-B5D8-94BFA8381274}" name="Jour"/>
+    <tableColumn id="6" xr3:uid="{36DFD9BF-E1E3-4A4A-87AE-14D902DA19FC}" name="Date/heure de début du match" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{395AEB18-E035-AF42-9143-1B22B2213A65}" name="Club recevant"/>
+    <tableColumn id="8" xr3:uid="{3E846188-E250-7648-A10B-91087C66A8F8}" name="Equipe recevante"/>
+    <tableColumn id="9" xr3:uid="{0E9F9FCD-D140-4240-9933-38EBF02976D9}" name="Equipe visiteuse"/>
+    <tableColumn id="10" xr3:uid="{7BBC4FE1-92E4-BD49-AD5A-AB0CD1385F20}" name="Salle"/>
+    <tableColumn id="11" xr3:uid="{F419F79C-A946-A940-B1E1-1E5EF059D731}" name="Equipe marqueur"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -769,15 +793,16 @@
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="20.1640625" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" customWidth="1"/>
-    <col min="10" max="10" width="36.83203125" customWidth="1"/>
-    <col min="11" max="11" width="26.83203125" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -3687,8 +3712,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:K83" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>